<commit_message>
Logger interface to ESP32 through special frame type and mutex access to logger
</commit_message>
<xml_diff>
--- a/Documentación/definición_tramas.xlsx
+++ b/Documentación/definición_tramas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>4bits</t>
   </si>
@@ -198,7 +198,16 @@
     <t xml:space="preserve">Raw data</t>
   </si>
   <si>
+    <t>logs</t>
+  </si>
+  <si>
     <t>0xD</t>
+  </si>
+  <si>
+    <t>&gt;0x002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON { logs:[ {"severity": number, "msg": string} ] }</t>
   </si>
   <si>
     <t>0xE</t>
@@ -335,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,11 +370,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1217,7 +1229,7 @@
       <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1229,10 +1241,10 @@
       <c r="F14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="3" t="s">
         <v>52</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -1249,7 +1261,7 @@
       <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1273,17 +1285,25 @@
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="B16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1291,7 +1311,7 @@
     <row r="17" ht="14.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1306,10 +1326,10 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
@@ -1375,7 +1395,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1389,7 +1409,7 @@
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1403,7 +1423,7 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1440,8 +1460,8 @@
       <c r="J27" s="3"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="14" t="s">
-        <v>68</v>
+      <c r="A28" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1455,7 +1475,7 @@
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1469,7 +1489,7 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1483,7 +1503,7 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1496,8 +1516,8 @@
       <c r="J31" s="3"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="15" t="s">
-        <v>72</v>
+      <c r="A32" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1510,8 +1530,8 @@
       <c r="J32" s="3"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="16" t="s">
-        <v>73</v>
+      <c r="A33" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1524,8 +1544,8 @@
       <c r="J33" s="3"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="17" t="s">
-        <v>74</v>
+      <c r="A34" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1538,9 +1558,10 @@
       <c r="J34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="E16:I16"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>